<commit_message>
Modelos escalados, implementacion 3er clasificador tipo 0 vs tipo 3, pruebas correctas
</commit_message>
<xml_diff>
--- a/resultado_clasificacion_unificado.xlsx
+++ b/resultado_clasificacion_unificado.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,22 +454,200 @@
           <t>tipo_plagio_predicho</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>sospecha_tipo3_%</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>porcentaje_tipo_plagio</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>codigo4.py</t>
+          <t>codigo1.py</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>codigo1.py</t>
+          <t>codigo4.py</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>codigo1.py</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>codigo4.py</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>codigo1.py</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>codigo4.py</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>34.92</v>
+      </c>
+      <c r="F4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>codigo1.py</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>codigo4.py</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>codigo1.py</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>codigo4.py</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>34.92</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>codigo1.py</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>codigo4.py</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>codigo1.py</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>codigo4.py</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>85.33</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>codigo1.py</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>codigo4.py</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>31.4</v>
+      </c>
+      <c r="F9" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>